<commit_message>
TanLoc_Commit11: Update dong goi api
</commit_message>
<xml_diff>
--- a/RFID_API/src/main/java/namviet/rfid_api/fileExport/file1.xlsx
+++ b/RFID_API/src/main/java/namviet/rfid_api/fileExport/file1.xlsx
@@ -35,13 +35,13 @@
     <t>Content 3</t>
   </si>
   <si>
-    <t>30300E890A0180C077359483</t>
+    <t>30300E890A0180C077359401</t>
   </si>
   <si>
     <t>00190517215391</t>
   </si>
   <si>
-    <t>2000000131</t>
+    <t>2000000001</t>
   </si>
   <si>
     <t>8935226670862</t>
@@ -53,778 +53,778 @@
     <t>PG 1 SUB 70 CR GRN</t>
   </si>
   <si>
-    <t>30300E890A0180C077359484</t>
-  </si>
-  <si>
-    <t>2000000132</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359485</t>
-  </si>
-  <si>
-    <t>2000000133</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359486</t>
-  </si>
-  <si>
-    <t>2000000134</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359487</t>
-  </si>
-  <si>
-    <t>2000000135</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359488</t>
-  </si>
-  <si>
-    <t>2000000136</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359489</t>
-  </si>
-  <si>
-    <t>2000000137</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948A</t>
-  </si>
-  <si>
-    <t>2000000138</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948B</t>
-  </si>
-  <si>
-    <t>2000000139</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948C</t>
-  </si>
-  <si>
-    <t>2000000140</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948D</t>
-  </si>
-  <si>
-    <t>2000000141</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948E</t>
-  </si>
-  <si>
-    <t>2000000142</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735948F</t>
-  </si>
-  <si>
-    <t>2000000143</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359490</t>
-  </si>
-  <si>
-    <t>2000000144</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359491</t>
-  </si>
-  <si>
-    <t>2000000145</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359492</t>
-  </si>
-  <si>
-    <t>2000000146</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359493</t>
-  </si>
-  <si>
-    <t>2000000147</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359494</t>
-  </si>
-  <si>
-    <t>2000000148</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359495</t>
-  </si>
-  <si>
-    <t>2000000149</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359496</t>
-  </si>
-  <si>
-    <t>2000000150</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359497</t>
-  </si>
-  <si>
-    <t>2000000151</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359498</t>
-  </si>
-  <si>
-    <t>2000000152</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359499</t>
-  </si>
-  <si>
-    <t>2000000153</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949A</t>
-  </si>
-  <si>
-    <t>2000000154</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949B</t>
-  </si>
-  <si>
-    <t>2000000155</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949C</t>
-  </si>
-  <si>
-    <t>2000000156</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949D</t>
-  </si>
-  <si>
-    <t>2000000157</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949E</t>
-  </si>
-  <si>
-    <t>2000000158</t>
-  </si>
-  <si>
-    <t>30300E890A0180C07735949F</t>
-  </si>
-  <si>
-    <t>2000000159</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A0</t>
-  </si>
-  <si>
-    <t>2000000160</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A1</t>
-  </si>
-  <si>
-    <t>2000000161</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A2</t>
-  </si>
-  <si>
-    <t>2000000162</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A3</t>
-  </si>
-  <si>
-    <t>2000000163</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A4</t>
-  </si>
-  <si>
-    <t>2000000164</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A5</t>
-  </si>
-  <si>
-    <t>2000000165</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A6</t>
-  </si>
-  <si>
-    <t>2000000166</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A7</t>
-  </si>
-  <si>
-    <t>2000000167</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A8</t>
-  </si>
-  <si>
-    <t>2000000168</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594A9</t>
-  </si>
-  <si>
-    <t>2000000169</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AA</t>
-  </si>
-  <si>
-    <t>2000000170</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AB</t>
-  </si>
-  <si>
-    <t>2000000171</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AC</t>
-  </si>
-  <si>
-    <t>2000000172</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AD</t>
-  </si>
-  <si>
-    <t>2000000173</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AE</t>
-  </si>
-  <si>
-    <t>2000000174</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594AF</t>
-  </si>
-  <si>
-    <t>2000000175</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B0</t>
-  </si>
-  <si>
-    <t>2000000176</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B1</t>
-  </si>
-  <si>
-    <t>2000000177</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B2</t>
-  </si>
-  <si>
-    <t>2000000178</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B3</t>
-  </si>
-  <si>
-    <t>2000000179</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B4</t>
-  </si>
-  <si>
-    <t>2000000180</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B5</t>
-  </si>
-  <si>
-    <t>2000000181</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B6</t>
-  </si>
-  <si>
-    <t>2000000182</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B7</t>
-  </si>
-  <si>
-    <t>2000000183</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B8</t>
-  </si>
-  <si>
-    <t>2000000184</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594B9</t>
-  </si>
-  <si>
-    <t>2000000185</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BA</t>
-  </si>
-  <si>
-    <t>2000000186</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BB</t>
-  </si>
-  <si>
-    <t>2000000187</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BC</t>
-  </si>
-  <si>
-    <t>2000000188</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BD</t>
-  </si>
-  <si>
-    <t>2000000189</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BE</t>
-  </si>
-  <si>
-    <t>2000000190</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594BF</t>
-  </si>
-  <si>
-    <t>2000000191</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C0</t>
-  </si>
-  <si>
-    <t>2000000192</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C1</t>
-  </si>
-  <si>
-    <t>2000000193</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C2</t>
-  </si>
-  <si>
-    <t>2000000194</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C3</t>
-  </si>
-  <si>
-    <t>2000000195</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C4</t>
-  </si>
-  <si>
-    <t>2000000196</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C5</t>
-  </si>
-  <si>
-    <t>2000000197</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C6</t>
-  </si>
-  <si>
-    <t>2000000198</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C7</t>
-  </si>
-  <si>
-    <t>2000000199</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C8</t>
-  </si>
-  <si>
-    <t>2000000200</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594C9</t>
-  </si>
-  <si>
-    <t>2000000201</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CA</t>
-  </si>
-  <si>
-    <t>2000000202</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CB</t>
-  </si>
-  <si>
-    <t>2000000203</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CC</t>
-  </si>
-  <si>
-    <t>2000000204</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CD</t>
-  </si>
-  <si>
-    <t>2000000205</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CE</t>
-  </si>
-  <si>
-    <t>2000000206</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594CF</t>
-  </si>
-  <si>
-    <t>2000000207</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D0</t>
-  </si>
-  <si>
-    <t>2000000208</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D1</t>
-  </si>
-  <si>
-    <t>2000000209</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D2</t>
-  </si>
-  <si>
-    <t>2000000210</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D3</t>
-  </si>
-  <si>
-    <t>2000000211</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D4</t>
-  </si>
-  <si>
-    <t>2000000212</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D5</t>
-  </si>
-  <si>
-    <t>2000000213</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D6</t>
-  </si>
-  <si>
-    <t>2000000214</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D7</t>
-  </si>
-  <si>
-    <t>2000000215</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D8</t>
-  </si>
-  <si>
-    <t>2000000216</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594D9</t>
-  </si>
-  <si>
-    <t>2000000217</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DA</t>
-  </si>
-  <si>
-    <t>2000000218</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DB</t>
-  </si>
-  <si>
-    <t>2000000219</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DC</t>
-  </si>
-  <si>
-    <t>2000000220</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DD</t>
-  </si>
-  <si>
-    <t>2000000221</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DE</t>
-  </si>
-  <si>
-    <t>2000000222</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594DF</t>
-  </si>
-  <si>
-    <t>2000000223</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E0</t>
-  </si>
-  <si>
-    <t>2000000224</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E1</t>
-  </si>
-  <si>
-    <t>2000000225</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E2</t>
-  </si>
-  <si>
-    <t>2000000226</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E3</t>
-  </si>
-  <si>
-    <t>2000000227</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E4</t>
-  </si>
-  <si>
-    <t>2000000228</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E5</t>
-  </si>
-  <si>
-    <t>2000000229</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E6</t>
-  </si>
-  <si>
-    <t>2000000230</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E7</t>
-  </si>
-  <si>
-    <t>2000000231</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E8</t>
-  </si>
-  <si>
-    <t>2000000232</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594E9</t>
-  </si>
-  <si>
-    <t>2000000233</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594EA</t>
-  </si>
-  <si>
-    <t>2000000234</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594EB</t>
-  </si>
-  <si>
-    <t>2000000235</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594EC</t>
-  </si>
-  <si>
-    <t>2000000236</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594ED</t>
-  </si>
-  <si>
-    <t>2000000237</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594EE</t>
-  </si>
-  <si>
-    <t>2000000238</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594EF</t>
-  </si>
-  <si>
-    <t>2000000239</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F0</t>
-  </si>
-  <si>
-    <t>2000000240</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F1</t>
-  </si>
-  <si>
-    <t>2000000241</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F2</t>
-  </si>
-  <si>
-    <t>2000000242</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F3</t>
-  </si>
-  <si>
-    <t>2000000243</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F4</t>
-  </si>
-  <si>
-    <t>2000000244</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F5</t>
-  </si>
-  <si>
-    <t>2000000245</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F6</t>
-  </si>
-  <si>
-    <t>2000000246</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F7</t>
-  </si>
-  <si>
-    <t>2000000247</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F8</t>
-  </si>
-  <si>
-    <t>2000000248</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594F9</t>
-  </si>
-  <si>
-    <t>2000000249</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FA</t>
-  </si>
-  <si>
-    <t>2000000250</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FB</t>
-  </si>
-  <si>
-    <t>2000000251</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FC</t>
-  </si>
-  <si>
-    <t>2000000252</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FD</t>
-  </si>
-  <si>
-    <t>2000000253</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FE</t>
-  </si>
-  <si>
-    <t>2000000254</t>
-  </si>
-  <si>
-    <t>30300E890A0180C0773594FF</t>
-  </si>
-  <si>
-    <t>2000000255</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359500</t>
-  </si>
-  <si>
-    <t>2000000256</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359501</t>
-  </si>
-  <si>
-    <t>2000000257</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359502</t>
-  </si>
-  <si>
-    <t>2000000258</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359503</t>
-  </si>
-  <si>
-    <t>2000000259</t>
-  </si>
-  <si>
-    <t>30300E890A0180C077359504</t>
-  </si>
-  <si>
-    <t>2000000260</t>
+    <t>30300E890A0180C077359402</t>
+  </si>
+  <si>
+    <t>2000000002</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359403</t>
+  </si>
+  <si>
+    <t>2000000003</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359404</t>
+  </si>
+  <si>
+    <t>2000000004</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359405</t>
+  </si>
+  <si>
+    <t>2000000005</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359406</t>
+  </si>
+  <si>
+    <t>2000000006</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359407</t>
+  </si>
+  <si>
+    <t>2000000007</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359408</t>
+  </si>
+  <si>
+    <t>2000000008</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359409</t>
+  </si>
+  <si>
+    <t>2000000009</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940A</t>
+  </si>
+  <si>
+    <t>2000000010</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940B</t>
+  </si>
+  <si>
+    <t>2000000011</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940C</t>
+  </si>
+  <si>
+    <t>2000000012</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940D</t>
+  </si>
+  <si>
+    <t>2000000013</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940E</t>
+  </si>
+  <si>
+    <t>2000000014</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735940F</t>
+  </si>
+  <si>
+    <t>2000000015</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359410</t>
+  </si>
+  <si>
+    <t>2000000016</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359411</t>
+  </si>
+  <si>
+    <t>2000000017</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359412</t>
+  </si>
+  <si>
+    <t>2000000018</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359413</t>
+  </si>
+  <si>
+    <t>2000000019</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359414</t>
+  </si>
+  <si>
+    <t>2000000020</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359415</t>
+  </si>
+  <si>
+    <t>2000000021</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359416</t>
+  </si>
+  <si>
+    <t>2000000022</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359417</t>
+  </si>
+  <si>
+    <t>2000000023</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359418</t>
+  </si>
+  <si>
+    <t>2000000024</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359419</t>
+  </si>
+  <si>
+    <t>2000000025</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941A</t>
+  </si>
+  <si>
+    <t>2000000026</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941B</t>
+  </si>
+  <si>
+    <t>2000000027</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941C</t>
+  </si>
+  <si>
+    <t>2000000028</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941D</t>
+  </si>
+  <si>
+    <t>2000000029</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941E</t>
+  </si>
+  <si>
+    <t>2000000030</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735941F</t>
+  </si>
+  <si>
+    <t>2000000031</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359420</t>
+  </si>
+  <si>
+    <t>2000000032</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359421</t>
+  </si>
+  <si>
+    <t>2000000033</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359422</t>
+  </si>
+  <si>
+    <t>2000000034</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359423</t>
+  </si>
+  <si>
+    <t>2000000035</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359424</t>
+  </si>
+  <si>
+    <t>2000000036</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359425</t>
+  </si>
+  <si>
+    <t>2000000037</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359426</t>
+  </si>
+  <si>
+    <t>2000000038</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359427</t>
+  </si>
+  <si>
+    <t>2000000039</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359428</t>
+  </si>
+  <si>
+    <t>2000000040</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359429</t>
+  </si>
+  <si>
+    <t>2000000041</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942A</t>
+  </si>
+  <si>
+    <t>2000000042</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942B</t>
+  </si>
+  <si>
+    <t>2000000043</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942C</t>
+  </si>
+  <si>
+    <t>2000000044</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942D</t>
+  </si>
+  <si>
+    <t>2000000045</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942E</t>
+  </si>
+  <si>
+    <t>2000000046</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735942F</t>
+  </si>
+  <si>
+    <t>2000000047</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359430</t>
+  </si>
+  <si>
+    <t>2000000048</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359431</t>
+  </si>
+  <si>
+    <t>2000000049</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359432</t>
+  </si>
+  <si>
+    <t>2000000050</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359433</t>
+  </si>
+  <si>
+    <t>2000000051</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359434</t>
+  </si>
+  <si>
+    <t>2000000052</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359435</t>
+  </si>
+  <si>
+    <t>2000000053</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359436</t>
+  </si>
+  <si>
+    <t>2000000054</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359437</t>
+  </si>
+  <si>
+    <t>2000000055</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359438</t>
+  </si>
+  <si>
+    <t>2000000056</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359439</t>
+  </si>
+  <si>
+    <t>2000000057</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943A</t>
+  </si>
+  <si>
+    <t>2000000058</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943B</t>
+  </si>
+  <si>
+    <t>2000000059</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943C</t>
+  </si>
+  <si>
+    <t>2000000060</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943D</t>
+  </si>
+  <si>
+    <t>2000000061</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943E</t>
+  </si>
+  <si>
+    <t>2000000062</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735943F</t>
+  </si>
+  <si>
+    <t>2000000063</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359440</t>
+  </si>
+  <si>
+    <t>2000000064</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359441</t>
+  </si>
+  <si>
+    <t>2000000065</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359442</t>
+  </si>
+  <si>
+    <t>2000000066</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359443</t>
+  </si>
+  <si>
+    <t>2000000067</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359444</t>
+  </si>
+  <si>
+    <t>2000000068</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359445</t>
+  </si>
+  <si>
+    <t>2000000069</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359446</t>
+  </si>
+  <si>
+    <t>2000000070</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359447</t>
+  </si>
+  <si>
+    <t>2000000071</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359448</t>
+  </si>
+  <si>
+    <t>2000000072</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359449</t>
+  </si>
+  <si>
+    <t>2000000073</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944A</t>
+  </si>
+  <si>
+    <t>2000000074</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944B</t>
+  </si>
+  <si>
+    <t>2000000075</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944C</t>
+  </si>
+  <si>
+    <t>2000000076</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944D</t>
+  </si>
+  <si>
+    <t>2000000077</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944E</t>
+  </si>
+  <si>
+    <t>2000000078</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735944F</t>
+  </si>
+  <si>
+    <t>2000000079</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359450</t>
+  </si>
+  <si>
+    <t>2000000080</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359451</t>
+  </si>
+  <si>
+    <t>2000000081</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359452</t>
+  </si>
+  <si>
+    <t>2000000082</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359453</t>
+  </si>
+  <si>
+    <t>2000000083</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359454</t>
+  </si>
+  <si>
+    <t>2000000084</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359455</t>
+  </si>
+  <si>
+    <t>2000000085</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359456</t>
+  </si>
+  <si>
+    <t>2000000086</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359457</t>
+  </si>
+  <si>
+    <t>2000000087</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359458</t>
+  </si>
+  <si>
+    <t>2000000088</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359459</t>
+  </si>
+  <si>
+    <t>2000000089</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945A</t>
+  </si>
+  <si>
+    <t>2000000090</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945B</t>
+  </si>
+  <si>
+    <t>2000000091</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945C</t>
+  </si>
+  <si>
+    <t>2000000092</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945D</t>
+  </si>
+  <si>
+    <t>2000000093</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945E</t>
+  </si>
+  <si>
+    <t>2000000094</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735945F</t>
+  </si>
+  <si>
+    <t>2000000095</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359460</t>
+  </si>
+  <si>
+    <t>2000000096</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359461</t>
+  </si>
+  <si>
+    <t>2000000097</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359462</t>
+  </si>
+  <si>
+    <t>2000000098</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359463</t>
+  </si>
+  <si>
+    <t>2000000099</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359464</t>
+  </si>
+  <si>
+    <t>2000000100</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359465</t>
+  </si>
+  <si>
+    <t>2000000101</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359466</t>
+  </si>
+  <si>
+    <t>2000000102</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359467</t>
+  </si>
+  <si>
+    <t>2000000103</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359468</t>
+  </si>
+  <si>
+    <t>2000000104</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359469</t>
+  </si>
+  <si>
+    <t>2000000105</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946A</t>
+  </si>
+  <si>
+    <t>2000000106</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946B</t>
+  </si>
+  <si>
+    <t>2000000107</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946C</t>
+  </si>
+  <si>
+    <t>2000000108</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946D</t>
+  </si>
+  <si>
+    <t>2000000109</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946E</t>
+  </si>
+  <si>
+    <t>2000000110</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735946F</t>
+  </si>
+  <si>
+    <t>2000000111</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359470</t>
+  </si>
+  <si>
+    <t>2000000112</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359471</t>
+  </si>
+  <si>
+    <t>2000000113</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359472</t>
+  </si>
+  <si>
+    <t>2000000114</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359473</t>
+  </si>
+  <si>
+    <t>2000000115</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359474</t>
+  </si>
+  <si>
+    <t>2000000116</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359475</t>
+  </si>
+  <si>
+    <t>2000000117</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359476</t>
+  </si>
+  <si>
+    <t>2000000118</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359477</t>
+  </si>
+  <si>
+    <t>2000000119</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359478</t>
+  </si>
+  <si>
+    <t>2000000120</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359479</t>
+  </si>
+  <si>
+    <t>2000000121</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947A</t>
+  </si>
+  <si>
+    <t>2000000122</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947B</t>
+  </si>
+  <si>
+    <t>2000000123</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947C</t>
+  </si>
+  <si>
+    <t>2000000124</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947D</t>
+  </si>
+  <si>
+    <t>2000000125</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947E</t>
+  </si>
+  <si>
+    <t>2000000126</t>
+  </si>
+  <si>
+    <t>30300E890A0180C07735947F</t>
+  </si>
+  <si>
+    <t>2000000127</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359480</t>
+  </si>
+  <si>
+    <t>2000000128</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359481</t>
+  </si>
+  <si>
+    <t>2000000129</t>
+  </si>
+  <si>
+    <t>30300E890A0180C077359482</t>
+  </si>
+  <si>
+    <t>2000000130</t>
   </si>
 </sst>
 </file>

</xml_diff>